<commit_message>
fixed getuser problem on RHEL/Centos
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests.xlsx
+++ b/elmclient/tests/tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3830B921-58AD-4EC2-A1F4-BCF75A81CA56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE10A3-1080-44F4-BB03-F70EB5CE0072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="45" windowWidth="25200" windowHeight="13695" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="-8430" yWindow="-21345" windowWidth="21600" windowHeight="11505" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>Logging</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>rdm_types:ArtifactFormat=jazz_rm:Collection</t>
   </si>
   <si>
@@ -706,6 +703,9 @@
   </si>
   <si>
     <t>ETM app query all streams (mutable) configurations</t>
+  </si>
+  <si>
+    <t>##########</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -832,6 +832,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1149,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
-  <dimension ref="A1:AF109"/>
+  <dimension ref="A1:AH109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,30 +1188,30 @@
     <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>31</v>
@@ -1217,22 +1220,22 @@
         <v>32</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>34</v>
@@ -1244,10 +1247,10 @@
         <v>35</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>10</v>
@@ -1265,36 +1268,36 @@
         <v>37</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1305,18 +1308,18 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="W2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -1326,10 +1329,11 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH3" s="17"/>
+    </row>
+    <row r="4" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5">
         <v>101</v>
@@ -1338,11 +1342,11 @@
         <v>738</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1380,22 +1384,25 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5">
         <f>C4+1</f>
         <v>102</v>
       </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>8</v>
@@ -1419,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="W5" s="5" t="str">
-        <f t="shared" ref="W5:Y44" si="1">W$2</f>
+        <f t="shared" ref="W5:X44" si="1">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X5" s="5" t="str">
@@ -1427,16 +1434,16 @@
         <v>ibm</v>
       </c>
       <c r="Y5" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ref="C6:C52" si="2">C5+1</f>
@@ -1478,16 +1485,16 @@
         <v>ibm</v>
       </c>
       <c r="Y6" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="2"/>
@@ -1509,16 +1516,16 @@
         <v>ibm</v>
       </c>
       <c r="Y7" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="2"/>
@@ -1543,23 +1550,26 @@
         <v>ibm</v>
       </c>
       <c r="Y8" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="2"/>
         <v>106</v>
       </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
       <c r="G9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>8</v>
@@ -1591,23 +1601,26 @@
         <v>ibm</v>
       </c>
       <c r="Y9" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
       <c r="G10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1636,23 +1649,26 @@
         <v>ibm</v>
       </c>
       <c r="Y10" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
       <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1681,23 +1697,26 @@
         <v>ibm</v>
       </c>
       <c r="Y11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="2"/>
         <v>109</v>
       </c>
+      <c r="F12" s="5">
+        <v>16</v>
+      </c>
       <c r="G12" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>0</v>
@@ -1731,13 +1750,13 @@
         <v>ibm</v>
       </c>
       <c r="Y12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="2"/>
@@ -1750,7 +1769,7 @@
         <v>19</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>0</v>
@@ -1784,16 +1803,16 @@
         <v>ibm</v>
       </c>
       <c r="Y13" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="2"/>
@@ -1803,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -1840,16 +1859,16 @@
         <v>ibm</v>
       </c>
       <c r="Y14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="2"/>
@@ -1862,7 +1881,7 @@
         <v>20</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>1</v>
@@ -1896,16 +1915,16 @@
         <v>ibm</v>
       </c>
       <c r="Y15" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="2"/>
@@ -1918,7 +1937,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>2</v>
@@ -1952,26 +1971,26 @@
         <v>ibm</v>
       </c>
       <c r="Y16" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="17" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2000,18 +2019,21 @@
         <v>ibm</v>
       </c>
       <c r="Y17" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
+      <c r="F18" s="5">
+        <v>738</v>
+      </c>
       <c r="G18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2042,18 +2064,21 @@
         <v>ibm</v>
       </c>
       <c r="Y18" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
+      <c r="F19" s="5">
+        <v>738</v>
+      </c>
       <c r="G19" s="5" t="s">
         <v>23</v>
       </c>
@@ -2084,13 +2109,13 @@
         <v>ibm</v>
       </c>
       <c r="Y19" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="20" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" si="2"/>
@@ -2132,13 +2157,13 @@
         <v>ibm</v>
       </c>
       <c r="Y20" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="21" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" si="2"/>
@@ -2148,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="M21" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2180,13 +2205,13 @@
         <v>ibm</v>
       </c>
       <c r="Y21" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" si="2"/>
@@ -2231,13 +2256,13 @@
         <v>ibm</v>
       </c>
       <c r="Y22" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="23" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" si="2"/>
@@ -2282,13 +2307,13 @@
         <v>ibm</v>
       </c>
       <c r="Y23" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="24" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" si="2"/>
@@ -2298,10 +2323,10 @@
         <v>148</v>
       </c>
       <c r="G24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="M24" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2330,13 +2355,13 @@
         <v>ibm</v>
       </c>
       <c r="Y24" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="25" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" si="2"/>
@@ -2346,10 +2371,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M25" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2379,16 +2404,16 @@
         <v>ibm</v>
       </c>
       <c r="Y25" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" si="2"/>
@@ -2398,10 +2423,10 @@
         <v>11</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M26" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2431,16 +2456,16 @@
         <v>ibm</v>
       </c>
       <c r="Y26" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="27" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" si="2"/>
@@ -2450,13 +2475,13 @@
         <v>708</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="J27" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M27" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2485,16 +2510,16 @@
         <v>ibm</v>
       </c>
       <c r="Y27" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="28" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" si="2"/>
@@ -2504,20 +2529,20 @@
         <v>354</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test125.csv</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -2544,16 +2569,16 @@
         <v>ibm</v>
       </c>
       <c r="Y28" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="29" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" si="2"/>
@@ -2563,20 +2588,20 @@
         <v>354</v>
       </c>
       <c r="G29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="M29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test126.csv</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>11</v>
@@ -2601,16 +2626,16 @@
         <v>ibm</v>
       </c>
       <c r="Y29" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="30" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" si="2"/>
@@ -2620,17 +2645,17 @@
         <v>733</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test127.csv</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
@@ -2657,13 +2682,13 @@
         <v>ibm</v>
       </c>
       <c r="Y30" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="31" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" s="5">
         <f t="shared" si="2"/>
@@ -2673,13 +2698,13 @@
         <v>12</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M31" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2708,13 +2733,13 @@
         <v>ibm</v>
       </c>
       <c r="Y31" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" si="2"/>
@@ -2724,13 +2749,13 @@
         <v>12</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M32" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2759,13 +2784,13 @@
         <v>ibm</v>
       </c>
       <c r="Y32" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="33" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="5">
         <f t="shared" si="2"/>
@@ -2775,10 +2800,10 @@
         <v>112</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M33" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2807,13 +2832,13 @@
         <v>ibm</v>
       </c>
       <c r="Y33" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="34" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="5">
         <f t="shared" si="2"/>
@@ -2823,17 +2848,17 @@
         <v>19</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test131.csv</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q34" s="5" t="s">
         <v>11</v>
@@ -2858,13 +2883,13 @@
         <v>ibm</v>
       </c>
       <c r="Y34" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="35" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="5">
         <f t="shared" si="2"/>
@@ -2874,17 +2899,17 @@
         <v>93</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>tests\results\test132.csv</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q35" s="5" t="s">
         <v>11</v>
@@ -2909,13 +2934,13 @@
         <v>ibm</v>
       </c>
       <c r="Y35" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="36" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" s="5">
         <f t="shared" si="2"/>
@@ -2925,7 +2950,7 @@
         <v>1476</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I36" s="8"/>
       <c r="M36" s="6" t="str">
@@ -2933,13 +2958,13 @@
         <v>tests\results\test133.csv</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T36" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="U36" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="U36" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="V36" s="5" t="s">
         <v>12</v>
@@ -2953,13 +2978,13 @@
         <v>ibm</v>
       </c>
       <c r="Y36" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="37" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="5">
         <f t="shared" si="2"/>
@@ -2969,7 +2994,7 @@
         <v>738</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I37" s="8"/>
       <c r="M37" s="6" t="str">
@@ -2977,13 +3002,13 @@
         <v>tests\results\test134.csv</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V37" s="5" t="s">
         <v>12</v>
@@ -2997,13 +3022,13 @@
         <v>ibm</v>
       </c>
       <c r="Y37" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="38" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="5">
         <f t="shared" si="2"/>
@@ -3013,7 +3038,7 @@
         <v>738</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I38" s="8"/>
       <c r="M38" s="6" t="str">
@@ -3021,13 +3046,13 @@
         <v>tests\results\test135.csv</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V38" s="5" t="s">
         <v>12</v>
@@ -3041,13 +3066,13 @@
         <v>ibm</v>
       </c>
       <c r="Y38" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="39" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="5">
         <f t="shared" si="2"/>
@@ -3057,11 +3082,11 @@
         <v>51</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I39" s="8"/>
       <c r="K39" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M39" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3090,13 +3115,13 @@
         <v>ibm</v>
       </c>
       <c r="Y39" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="40" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="5">
         <f t="shared" si="2"/>
@@ -3106,16 +3131,16 @@
         <v>112</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M40" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3144,13 +3169,13 @@
         <v>ibm</v>
       </c>
       <c r="Y40" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="41" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="5">
         <f t="shared" si="2"/>
@@ -3160,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I41" s="8"/>
       <c r="L41" s="6"/>
@@ -3194,13 +3219,13 @@
         <v>ibm</v>
       </c>
       <c r="Y41" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="42" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="5">
         <f t="shared" si="2"/>
@@ -3210,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" s="8"/>
       <c r="L42" s="6"/>
@@ -3244,13 +3269,13 @@
         <v>ibm</v>
       </c>
       <c r="Y42" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="43" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" si="2"/>
@@ -3260,10 +3285,10 @@
         <v>5</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I43" s="8"/>
       <c r="L43" s="6"/>
@@ -3294,13 +3319,13 @@
         <v>ibm</v>
       </c>
       <c r="Y43" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="44" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="5">
         <f t="shared" si="2"/>
@@ -3310,7 +3335,7 @@
         <v>1652</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I44" s="8"/>
       <c r="M44" s="6" t="str">
@@ -3318,13 +3343,13 @@
         <v>tests\results\test141.csv</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V44" s="5" t="s">
         <v>12</v>
@@ -3338,13 +3363,13 @@
         <v>ibm</v>
       </c>
       <c r="Y44" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="45" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="5">
         <f t="shared" si="2"/>
@@ -3354,7 +3379,7 @@
         <v>325</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I45" s="8"/>
       <c r="M45" s="6" t="str">
@@ -3362,13 +3387,13 @@
         <v>tests\results\test142.csv</v>
       </c>
       <c r="Q45" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="S45" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="R45" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>12</v>
@@ -3382,13 +3407,13 @@
         <v>ibm</v>
       </c>
       <c r="Y45" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="46" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="5">
         <f t="shared" si="2"/>
@@ -3398,7 +3423,7 @@
         <v>744</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I46" s="8"/>
       <c r="M46" s="6" t="str">
@@ -3406,13 +3431,13 @@
         <v>tests\results\test143.csv</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V46" s="5" t="s">
         <v>12</v>
@@ -3426,13 +3451,13 @@
         <v>ibm</v>
       </c>
       <c r="Y46" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="47" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="5">
         <f t="shared" si="2"/>
@@ -3442,7 +3467,7 @@
         <v>583</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I47" s="8"/>
       <c r="M47" s="6" t="str">
@@ -3450,18 +3475,18 @@
         <v>tests\results\test144.csv</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S47" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="5">
         <f t="shared" si="2"/>
@@ -3471,10 +3496,10 @@
         <v>92</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>8</v>
@@ -3507,13 +3532,13 @@
         <v>ibm</v>
       </c>
       <c r="Y48" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="49" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="5">
         <f t="shared" si="2"/>
@@ -3523,10 +3548,10 @@
         <v>62</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>8</v>
@@ -3559,13 +3584,13 @@
         <v>ibm</v>
       </c>
       <c r="Y49" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="50" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="5">
         <f t="shared" si="2"/>
@@ -3575,10 +3600,10 @@
         <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>8</v>
@@ -3611,13 +3636,13 @@
         <v>ibm</v>
       </c>
       <c r="Y50" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="51" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="5">
         <f t="shared" si="2"/>
@@ -3627,10 +3652,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>8</v>
@@ -3663,13 +3688,13 @@
         <v>ibm</v>
       </c>
       <c r="Y51" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="52" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="5">
         <f t="shared" si="2"/>
@@ -3679,10 +3704,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>8</v>
@@ -3715,31 +3740,31 @@
         <v>ibm</v>
       </c>
       <c r="Y52" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="9">
         <v>201</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F56" s="9">
         <v>15</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>8</v>
@@ -3757,29 +3782,29 @@
         <v>ibm</v>
       </c>
       <c r="Y56" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="9">
         <f>C56+1</f>
         <v>202</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F57" s="9">
         <v>9</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M57" s="13" t="str">
         <f t="shared" si="46"/>
@@ -3794,26 +3819,26 @@
         <v>ibm</v>
       </c>
       <c r="Y57" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="9">
         <f t="shared" ref="C58:C63" si="48">C57+1</f>
         <v>203</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F58" s="9">
         <v>3</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>35</v>
@@ -3831,39 +3856,39 @@
         <v>ibm</v>
       </c>
       <c r="Y58" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="59" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="9">
         <f t="shared" si="48"/>
         <v>204</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F59" s="9">
         <v>30</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M59" s="13" t="str">
         <f t="shared" ref="M59:M60" si="50">"tests\results\test"&amp;C59&amp;".csv"</f>
         <v>tests\results\test204.csv</v>
       </c>
       <c r="Q59" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R59" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S59" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R59" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S59" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W59" s="9" t="str">
         <f t="shared" si="47"/>
@@ -3874,45 +3899,45 @@
         <v>ibm</v>
       </c>
       <c r="Y59" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA59" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C60" s="9">
         <f t="shared" si="48"/>
         <v>205</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F60" s="9">
         <v>4</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M60" s="13" t="str">
         <f t="shared" si="50"/>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R60" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S60" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R60" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S60" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W60" s="9" t="str">
         <f t="shared" si="47"/>
@@ -3923,42 +3948,42 @@
         <v>ibm</v>
       </c>
       <c r="Y60" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C61" s="9">
         <f t="shared" si="48"/>
         <v>206</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F61" s="9">
         <v>27</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M61" s="13" t="str">
         <f>"tests\results\test"&amp;C60&amp;".csv"</f>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q61" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S61" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R61" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S61" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W61" s="9" t="str">
         <f t="shared" si="47"/>
@@ -3969,42 +3994,42 @@
         <v>ibm</v>
       </c>
       <c r="Y61" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="62" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62" s="9">
         <f t="shared" si="48"/>
         <v>207</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F62" s="9">
         <v>22</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M62" s="13" t="str">
         <f>"tests\results\test"&amp;C61&amp;".csv"</f>
         <v>tests\results\test206.csv</v>
       </c>
       <c r="N62" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q62" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S62" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R62" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S62" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W62" s="9" t="str">
         <f t="shared" si="47"/>
@@ -4015,42 +4040,42 @@
         <v>ibm</v>
       </c>
       <c r="Y62" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="63" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C63" s="9">
         <f t="shared" si="48"/>
         <v>208</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F63" s="9">
         <v>8</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M63" s="13" t="str">
         <f>"tests\results\test"&amp;C62&amp;".csv"</f>
         <v>tests\results\test207.csv</v>
       </c>
       <c r="P63" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q63" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S63" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R63" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S63" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W63" s="9" t="str">
         <f t="shared" si="47"/>
@@ -4061,20 +4086,20 @@
         <v>ibm</v>
       </c>
       <c r="Y63" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="64" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M64" s="13"/>
       <c r="Q64" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S64" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R64" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S64" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W64" s="9" t="str">
         <f t="shared" si="47"/>
@@ -4085,20 +4110,20 @@
         <v>ibm</v>
       </c>
       <c r="Y64" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="65" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M65" s="13"/>
       <c r="Q65" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S65" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="R65" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="S65" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="W65" s="9" t="str">
         <f t="shared" si="47"/>
@@ -4109,31 +4134,31 @@
         <v>ibm</v>
       </c>
       <c r="Y65" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" s="4">
         <v>301</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F69" s="4">
         <v>89</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>8</v>
@@ -4143,7 +4168,7 @@
         <v>tests\results\test301.csv</v>
       </c>
       <c r="Q69" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W69" s="4" t="str">
         <f t="shared" ref="W69:Y84" si="52">W$2</f>
@@ -4154,32 +4179,32 @@
         <v>ibm</v>
       </c>
       <c r="Y69" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA69" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C70" s="4">
         <f>C69+1</f>
         <v>302</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F70" s="4">
         <v>34</v>
       </c>
       <c r="G70" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I70" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>8</v>
@@ -4189,7 +4214,7 @@
         <v>tests\results\test302.csv</v>
       </c>
       <c r="Q70" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W70" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4200,29 +4225,29 @@
         <v>ibm</v>
       </c>
       <c r="Y70" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="71" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" s="4">
         <f t="shared" ref="C71:C80" si="53">C70+1</f>
         <v>303</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F71" s="4">
         <v>23</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>8</v>
@@ -4232,7 +4257,7 @@
         <v>tests\results\test303.csv</v>
       </c>
       <c r="Q71" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W71" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4243,29 +4268,29 @@
         <v>ibm</v>
       </c>
       <c r="Y71" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="72" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72" s="4">
         <f t="shared" si="53"/>
         <v>304</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F72" s="4">
         <v>2</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>8</v>
@@ -4275,7 +4300,7 @@
         <v>tests\results\test304.csv</v>
       </c>
       <c r="Q72" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W72" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4286,39 +4311,39 @@
         <v>ibm</v>
       </c>
       <c r="Y72" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="73" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="4">
         <f t="shared" si="53"/>
         <v>305</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F73" s="4">
         <v>12</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M73" s="11" t="str">
         <f t="shared" si="51"/>
         <v>tests\results\test305.csv</v>
       </c>
       <c r="Q73" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W73" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4329,29 +4354,29 @@
         <v>ibm</v>
       </c>
       <c r="Y73" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="74" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C74" s="4">
         <f t="shared" si="53"/>
         <v>306</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F74" s="4">
         <v>89</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>8</v>
@@ -4361,7 +4386,7 @@
         <v>tests\results\test306.csv</v>
       </c>
       <c r="Q74" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W74" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4372,29 +4397,29 @@
         <v>ibm</v>
       </c>
       <c r="Y74" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="75" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" s="4">
         <f t="shared" si="53"/>
         <v>307</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F75" s="4">
         <v>0</v>
       </c>
       <c r="G75" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I75" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>8</v>
@@ -4404,7 +4429,7 @@
         <v>tests\results\test307.csv</v>
       </c>
       <c r="Q75" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W75" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4415,26 +4440,26 @@
         <v>ibm</v>
       </c>
       <c r="Y75" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="76" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="4">
         <f t="shared" si="53"/>
         <v>308</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F76" s="4">
         <v>23</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>8</v>
@@ -4444,10 +4469,10 @@
         <v>tests\results\test308.csv</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q76" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W76" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4458,26 +4483,26 @@
         <v>ibm</v>
       </c>
       <c r="Y76" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="77" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C77" s="4">
         <f t="shared" si="53"/>
         <v>309</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F77" s="4">
         <v>66</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>8</v>
@@ -4487,10 +4512,10 @@
         <v>tests\results\test309.csv</v>
       </c>
       <c r="P77" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q77" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W77" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4501,29 +4526,29 @@
         <v>ibm</v>
       </c>
       <c r="Y77" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="78" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C78" s="4">
         <f t="shared" si="53"/>
         <v>310</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F78" s="4">
         <v>38</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>8</v>
@@ -4533,7 +4558,7 @@
         <v>tests\results\test310.csv</v>
       </c>
       <c r="Q78" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W78" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4544,36 +4569,36 @@
         <v>ibm</v>
       </c>
       <c r="Y78" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="79" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="4">
         <f t="shared" si="53"/>
         <v>311</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F79" s="4">
         <v>2</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M79" s="11" t="str">
         <f t="shared" si="54"/>
         <v>tests\results\test311.csv</v>
       </c>
       <c r="Q79" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W79" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4584,26 +4609,26 @@
         <v>ibm</v>
       </c>
       <c r="Y79" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="80" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="4">
         <f t="shared" si="53"/>
         <v>312</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F80" s="4">
         <v>1</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>8</v>
@@ -4613,10 +4638,10 @@
         <v>tests\results\test312.csv</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q80" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W80" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4627,17 +4652,17 @@
         <v>ibm</v>
       </c>
       <c r="Y80" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA80" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M81" s="11"/>
       <c r="Q81" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W81" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4648,14 +4673,14 @@
         <v>ibm</v>
       </c>
       <c r="Y81" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="82" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M82" s="11"/>
       <c r="Q82" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W82" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4666,14 +4691,14 @@
         <v>ibm</v>
       </c>
       <c r="Y82" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="83" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M83" s="11"/>
       <c r="Q83" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W83" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4684,14 +4709,14 @@
         <v>ibm</v>
       </c>
       <c r="Y83" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="84" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M84" s="11"/>
       <c r="Q84" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W84" s="4" t="str">
         <f t="shared" si="52"/>
@@ -4702,7 +4727,7 @@
         <v>ibm</v>
       </c>
       <c r="Y84" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4711,24 +4736,24 @@
     </row>
     <row r="87" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C88" s="3">
         <v>401</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F88" s="3">
         <v>26</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>36</v>
@@ -4749,26 +4774,26 @@
         <v>ibm</v>
       </c>
       <c r="Y88" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C89" s="3">
         <f>C88+1</f>
         <v>402</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F89" s="3">
         <v>5</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>35</v>
@@ -4789,26 +4814,26 @@
         <v>ibm</v>
       </c>
       <c r="Y89" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="90" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C90" s="3">
         <f t="shared" ref="C90:C92" si="58">C89+1</f>
         <v>403</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F90" s="3">
         <v>4</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>35</v>
@@ -4821,7 +4846,7 @@
         <v>tests\results\test403.csv</v>
       </c>
       <c r="Q90" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W90" s="3" t="str">
         <f t="shared" si="56"/>
@@ -4832,29 +4857,29 @@
         <v>ibm</v>
       </c>
       <c r="Y90" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA90" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C91" s="3">
         <f t="shared" si="58"/>
         <v>404</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F91" s="3">
         <v>24</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>36</v>
@@ -4867,13 +4892,13 @@
         <v>tests\results\test404.csv</v>
       </c>
       <c r="Q91" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R91" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R91" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="S91" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="W91" s="3" t="str">
         <f t="shared" si="56"/>
@@ -4884,32 +4909,32 @@
         <v>ibm</v>
       </c>
       <c r="Y91" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C92" s="3">
         <f t="shared" si="58"/>
         <v>405</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F92" s="3">
         <v>1</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>35</v>
       </c>
       <c r="I92" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>8</v>
@@ -4919,7 +4944,7 @@
         <v>tests\results\test405.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W92" s="3" t="str">
         <f t="shared" si="56"/>
@@ -4930,7 +4955,7 @@
         <v>ibm</v>
       </c>
       <c r="Y92" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4939,10 +4964,10 @@
     <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G97" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I97" s="15"/>
       <c r="J97" s="15"/>
@@ -4956,13 +4981,13 @@
     </row>
     <row r="98" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C98" s="14">
         <v>1001</v>
       </c>
       <c r="G98" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I98" s="15"/>
       <c r="J98" s="15"/>
@@ -4996,12 +5021,12 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AB98" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C99" s="14">
         <f>C98+1</f>
@@ -5011,7 +5036,7 @@
         <v>738</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
@@ -5033,31 +5058,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W99" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X99" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X99" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y99" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC99" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C100" s="14">
         <f t="shared" ref="C100:C107" si="62">C99+1</f>
         <v>1003</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
@@ -5079,31 +5104,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W100" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X100" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X100" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y100" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC100" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE100" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C101" s="14">
         <f t="shared" si="62"/>
         <v>1004</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
@@ -5125,31 +5150,31 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X101" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X101" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y101" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AD101" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C102" s="14">
         <f t="shared" si="62"/>
         <v>1005</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
@@ -5171,28 +5196,28 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X102" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X102" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y102" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC102" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C103" s="14">
         <f t="shared" si="62"/>
         <v>1006</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I103" s="15"/>
       <c r="J103" s="15"/>
@@ -5226,22 +5251,22 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AB103" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE103" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C104" s="14">
         <f t="shared" si="62"/>
         <v>1007</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I104" s="15"/>
       <c r="J104" s="15"/>
@@ -5263,34 +5288,34 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W104" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X104" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X104" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y104" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC104" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE104" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C105" s="14">
         <f t="shared" si="62"/>
         <v>1008</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
@@ -5312,34 +5337,34 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W105" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X105" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X105" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y105" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC105" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE105" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C106" s="14">
         <f t="shared" si="62"/>
         <v>1009</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
@@ -5361,28 +5386,28 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X106" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X106" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y106" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AC106" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C107" s="14">
         <f t="shared" si="62"/>
         <v>1010</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -5404,16 +5429,16 @@
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X107" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="X107" s="14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y107" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AD107" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5440,7 +5465,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{5564B6BC-4AEC-446D-B468-A6617112B7EA}"/>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{2ACC8BDC-C889-4943-94E4-152B5ED32C84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Added represt, fixed reqif_io, many other little changes
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests.xlsx
+++ b/elmclient/tests/tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE10A3-1080-44F4-BB03-F70EB5CE0072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013CD760-4CE2-49D6-B1A2-F306A947FD2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8430" yWindow="-21345" windowWidth="21600" windowHeight="11505" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="15060" yWindow="-20760" windowWidth="29655" windowHeight="16050" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="227">
   <si>
     <t>oslc_rm:uses</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>##########</t>
+  </si>
+  <si>
+    <t>rm,gc</t>
   </si>
 </sst>
 </file>
@@ -1154,9 +1157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
   <dimension ref="A1:AH109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH3" sqref="AH3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1437,7 @@
         <v>ibm</v>
       </c>
       <c r="Y5" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" ref="Y5:Y46" si="2">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1446,7 +1449,7 @@
         <v>82</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" ref="C6:C52" si="2">C5+1</f>
+        <f t="shared" ref="C6:C52" si="3">C5+1</f>
         <v>103</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -1466,11 +1469,11 @@
         <v>11</v>
       </c>
       <c r="R6" s="5" t="str">
-        <f t="shared" ref="R6:R23" si="3">Q6&amp;" Initial Stream"</f>
+        <f t="shared" ref="R6:R23" si="4">Q6&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S6" s="5" t="str">
-        <f t="shared" ref="S6:S23" si="4">Q6</f>
+        <f t="shared" ref="S6:S23" si="5">Q6</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V6" s="5" t="s">
@@ -1485,7 +1488,7 @@
         <v>ibm</v>
       </c>
       <c r="Y6" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1497,7 +1500,7 @@
         <v>82</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -1516,7 +1519,7 @@
         <v>ibm</v>
       </c>
       <c r="Y7" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1528,7 +1531,7 @@
         <v>82</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -1550,7 +1553,7 @@
         <v>ibm</v>
       </c>
       <c r="Y8" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1559,7 +1562,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="F9" s="5">
@@ -1582,11 +1585,11 @@
         <v>11</v>
       </c>
       <c r="R9" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S9" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V9" s="5" t="s">
@@ -1601,7 +1604,7 @@
         <v>ibm</v>
       </c>
       <c r="Y9" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1610,7 +1613,7 @@
         <v>82</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="F10" s="5">
@@ -1630,11 +1633,11 @@
         <v>11</v>
       </c>
       <c r="R10" s="5" t="str">
-        <f t="shared" ref="R10" si="5">Q10&amp;" Initial Stream"</f>
+        <f t="shared" ref="R10" si="6">Q10&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S10" s="5" t="str">
-        <f t="shared" ref="S10" si="6">Q10</f>
+        <f t="shared" ref="S10" si="7">Q10</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V10" s="5" t="s">
@@ -1649,7 +1652,7 @@
         <v>ibm</v>
       </c>
       <c r="Y10" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1658,7 +1661,7 @@
         <v>82</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="F11" s="5">
@@ -1678,11 +1681,11 @@
         <v>11</v>
       </c>
       <c r="R11" s="5" t="str">
-        <f t="shared" ref="R11" si="7">Q11&amp;" Initial Stream"</f>
+        <f t="shared" ref="R11" si="8">Q11&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S11" s="5" t="str">
-        <f t="shared" ref="S11" si="8">Q11</f>
+        <f t="shared" ref="S11" si="9">Q11</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V11" s="5" t="s">
@@ -1697,7 +1700,7 @@
         <v>ibm</v>
       </c>
       <c r="Y11" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1706,7 +1709,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="F12" s="5">
@@ -1731,11 +1734,11 @@
         <v>11</v>
       </c>
       <c r="R12" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S12" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V12" s="5" t="s">
@@ -1750,7 +1753,7 @@
         <v>ibm</v>
       </c>
       <c r="Y12" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1759,7 +1762,7 @@
         <v>82</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="F13" s="5">
@@ -1784,11 +1787,11 @@
         <v>11</v>
       </c>
       <c r="R13" s="5" t="str">
-        <f t="shared" ref="R13" si="9">Q13&amp;" Initial Stream"</f>
+        <f t="shared" ref="R13" si="10">Q13&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S13" s="5" t="str">
-        <f t="shared" ref="S13" si="10">Q13</f>
+        <f t="shared" ref="S13" si="11">Q13</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V13" s="5" t="s">
@@ -1803,7 +1806,7 @@
         <v>ibm</v>
       </c>
       <c r="Y13" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1815,7 +1818,7 @@
         <v>184</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="F14" s="5">
@@ -1840,11 +1843,11 @@
         <v>11</v>
       </c>
       <c r="R14" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S14" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V14" s="5" t="s">
@@ -1859,7 +1862,7 @@
         <v>ibm</v>
       </c>
       <c r="Y14" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1871,7 +1874,7 @@
         <v>184</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="F15" s="5">
@@ -1896,11 +1899,11 @@
         <v>11</v>
       </c>
       <c r="R15" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S15" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V15" s="5" t="s">
@@ -1915,7 +1918,7 @@
         <v>ibm</v>
       </c>
       <c r="Y15" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1927,7 +1930,7 @@
         <v>184</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="F16" s="5">
@@ -1952,11 +1955,11 @@
         <v>11</v>
       </c>
       <c r="R16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S16" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V16" s="5" t="s">
@@ -1971,7 +1974,7 @@
         <v>ibm</v>
       </c>
       <c r="Y16" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -1983,7 +1986,7 @@
         <v>82</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -2000,11 +2003,11 @@
         <v>11</v>
       </c>
       <c r="R17" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S17" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V17" s="5" t="s">
@@ -2019,7 +2022,7 @@
         <v>ibm</v>
       </c>
       <c r="Y17" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2028,7 +2031,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="F18" s="5">
@@ -2045,11 +2048,11 @@
         <v>11</v>
       </c>
       <c r="R18" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S18" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V18" s="5" t="s">
@@ -2064,7 +2067,7 @@
         <v>ibm</v>
       </c>
       <c r="Y18" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2073,7 +2076,7 @@
         <v>82</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="F19" s="5">
@@ -2090,11 +2093,11 @@
         <v>11</v>
       </c>
       <c r="R19" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S19" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V19" s="5" t="s">
@@ -2109,7 +2112,7 @@
         <v>ibm</v>
       </c>
       <c r="Y19" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2118,7 +2121,7 @@
         <v>82</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="F20" s="5">
@@ -2138,11 +2141,11 @@
         <v>11</v>
       </c>
       <c r="R20" s="5" t="str">
-        <f t="shared" ref="R20" si="11">Q20&amp;" Initial Stream"</f>
+        <f t="shared" ref="R20" si="12">Q20&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S20" s="5" t="str">
-        <f t="shared" ref="S20" si="12">Q20</f>
+        <f t="shared" ref="S20" si="13">Q20</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V20" s="5" t="s">
@@ -2157,7 +2160,7 @@
         <v>ibm</v>
       </c>
       <c r="Y20" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2166,7 +2169,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="F21" s="5">
@@ -2186,11 +2189,11 @@
         <v>11</v>
       </c>
       <c r="R21" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S21" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V21" s="5" t="s">
@@ -2205,7 +2208,7 @@
         <v>ibm</v>
       </c>
       <c r="Y21" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2214,7 +2217,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="F22" s="5">
@@ -2237,11 +2240,11 @@
         <v>11</v>
       </c>
       <c r="R22" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S22" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V22" s="5" t="s">
@@ -2256,7 +2259,7 @@
         <v>ibm</v>
       </c>
       <c r="Y22" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2265,7 +2268,7 @@
         <v>82</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="F23" s="5">
@@ -2288,11 +2291,11 @@
         <v>11</v>
       </c>
       <c r="R23" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S23" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V23" s="5" t="s">
@@ -2307,7 +2310,7 @@
         <v>ibm</v>
       </c>
       <c r="Y23" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2316,7 +2319,7 @@
         <v>82</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="F24" s="5">
@@ -2336,11 +2339,11 @@
         <v>11</v>
       </c>
       <c r="R24" s="5" t="str">
-        <f t="shared" ref="R24:R25" si="13">Q24&amp;" Initial Stream"</f>
+        <f t="shared" ref="R24:R25" si="14">Q24&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S24" s="5" t="str">
-        <f t="shared" ref="S24:S25" si="14">Q24</f>
+        <f t="shared" ref="S24:S25" si="15">Q24</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V24" s="5" t="s">
@@ -2355,7 +2358,7 @@
         <v>ibm</v>
       </c>
       <c r="Y24" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2364,7 +2367,7 @@
         <v>82</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="F25" s="5">
@@ -2385,11 +2388,11 @@
         <v>11</v>
       </c>
       <c r="R25" s="5" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S25" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V25" s="5" t="s">
@@ -2404,7 +2407,7 @@
         <v>ibm</v>
       </c>
       <c r="Y25" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2416,7 +2419,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="F26" s="5">
@@ -2437,11 +2440,11 @@
         <v>11</v>
       </c>
       <c r="R26" s="5" t="str">
-        <f t="shared" ref="R26:R30" si="15">Q26&amp;" Initial Stream"</f>
+        <f t="shared" ref="R26:R30" si="16">Q26&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S26" s="5" t="str">
-        <f t="shared" ref="S26:S30" si="16">Q26</f>
+        <f t="shared" ref="S26:S30" si="17">Q26</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V26" s="5" t="s">
@@ -2456,7 +2459,7 @@
         <v>ibm</v>
       </c>
       <c r="Y26" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2468,7 +2471,7 @@
         <v>82</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="F27" s="5">
@@ -2491,11 +2494,11 @@
         <v>11</v>
       </c>
       <c r="R27" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S27" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V27" s="5" t="s">
@@ -2510,7 +2513,7 @@
         <v>ibm</v>
       </c>
       <c r="Y27" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2522,7 +2525,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="F28" s="5">
@@ -2550,11 +2553,11 @@
         <v>11</v>
       </c>
       <c r="R28" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S28" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V28" s="5" t="s">
@@ -2569,7 +2572,7 @@
         <v>ibm</v>
       </c>
       <c r="Y28" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2581,7 +2584,7 @@
         <v>82</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="F29" s="5">
@@ -2607,11 +2610,11 @@
         <v>11</v>
       </c>
       <c r="R29" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S29" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V29" s="5" t="s">
@@ -2626,7 +2629,7 @@
         <v>ibm</v>
       </c>
       <c r="Y29" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2638,7 +2641,7 @@
         <v>82</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="F30" s="5">
@@ -2663,11 +2666,11 @@
         <v>11</v>
       </c>
       <c r="R30" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S30" s="5" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V30" s="5" t="s">
@@ -2682,7 +2685,7 @@
         <v>ibm</v>
       </c>
       <c r="Y30" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2691,7 +2694,7 @@
         <v>82</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="F31" s="5">
@@ -2714,11 +2717,11 @@
         <v>11</v>
       </c>
       <c r="R31" s="5" t="str">
-        <f t="shared" ref="R31:R32" si="17">Q31&amp;" Initial Stream"</f>
+        <f t="shared" ref="R31:R32" si="18">Q31&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S31" s="5" t="str">
-        <f t="shared" ref="S31:S32" si="18">Q31</f>
+        <f t="shared" ref="S31:S32" si="19">Q31</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V31" s="5" t="s">
@@ -2733,7 +2736,7 @@
         <v>ibm</v>
       </c>
       <c r="Y31" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2742,7 +2745,7 @@
         <v>82</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="F32" s="5">
@@ -2765,11 +2768,11 @@
         <v>11</v>
       </c>
       <c r="R32" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S32" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V32" s="5" t="s">
@@ -2784,7 +2787,7 @@
         <v>ibm</v>
       </c>
       <c r="Y32" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2793,7 +2796,7 @@
         <v>82</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="F33" s="5">
@@ -2813,11 +2816,11 @@
         <v>11</v>
       </c>
       <c r="R33" s="5" t="str">
-        <f t="shared" ref="R33:R35" si="19">Q33&amp;" Initial Stream"</f>
+        <f t="shared" ref="R33:R35" si="20">Q33&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S33" s="5" t="str">
-        <f t="shared" ref="S33:S35" si="20">Q33</f>
+        <f t="shared" ref="S33:S35" si="21">Q33</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V33" s="5" t="s">
@@ -2832,7 +2835,7 @@
         <v>ibm</v>
       </c>
       <c r="Y33" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2841,7 +2844,7 @@
         <v>82</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="F34" s="5">
@@ -2864,11 +2867,11 @@
         <v>11</v>
       </c>
       <c r="R34" s="5" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S34" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V34" s="5" t="s">
@@ -2883,7 +2886,7 @@
         <v>ibm</v>
       </c>
       <c r="Y34" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2892,7 +2895,7 @@
         <v>82</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="F35" s="5">
@@ -2915,11 +2918,11 @@
         <v>11</v>
       </c>
       <c r="R35" s="5" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S35" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V35" s="5" t="s">
@@ -2934,7 +2937,7 @@
         <v>ibm</v>
       </c>
       <c r="Y35" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2943,8 +2946,11 @@
         <v>82</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="F36" s="5">
         <v>1476</v>
@@ -2978,7 +2984,7 @@
         <v>ibm</v>
       </c>
       <c r="Y36" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -2987,7 +2993,7 @@
         <v>82</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134</v>
       </c>
       <c r="F37" s="5">
@@ -2998,7 +3004,7 @@
       </c>
       <c r="I37" s="8"/>
       <c r="M37" s="6" t="str">
-        <f t="shared" ref="M37:M38" si="21">"tests\results\test"&amp;C37&amp;".csv"</f>
+        <f t="shared" ref="M37:M38" si="22">"tests\results\test"&amp;C37&amp;".csv"</f>
         <v>tests\results\test134.csv</v>
       </c>
       <c r="Q37" s="5" t="s">
@@ -3022,7 +3028,7 @@
         <v>ibm</v>
       </c>
       <c r="Y37" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3031,7 +3037,7 @@
         <v>82</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="F38" s="5">
@@ -3042,7 +3048,7 @@
       </c>
       <c r="I38" s="8"/>
       <c r="M38" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>tests\results\test135.csv</v>
       </c>
       <c r="Q38" s="5" t="s">
@@ -3066,7 +3072,7 @@
         <v>ibm</v>
       </c>
       <c r="Y38" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3075,7 +3081,7 @@
         <v>82</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="F39" s="5">
@@ -3096,11 +3102,11 @@
         <v>11</v>
       </c>
       <c r="R39" s="5" t="str">
-        <f t="shared" ref="R39:R40" si="22">Q39&amp;" Initial Stream"</f>
+        <f t="shared" ref="R39:R40" si="23">Q39&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S39" s="5" t="str">
-        <f t="shared" ref="S39:S40" si="23">Q39</f>
+        <f t="shared" ref="S39:S40" si="24">Q39</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V39" s="5" t="s">
@@ -3115,7 +3121,7 @@
         <v>ibm</v>
       </c>
       <c r="Y39" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3124,7 +3130,7 @@
         <v>82</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="F40" s="5">
@@ -3150,11 +3156,11 @@
         <v>11</v>
       </c>
       <c r="R40" s="5" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S40" s="5" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V40" s="5" t="s">
@@ -3169,7 +3175,7 @@
         <v>ibm</v>
       </c>
       <c r="Y40" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3178,7 +3184,7 @@
         <v>82</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="F41" s="5">
@@ -3200,11 +3206,11 @@
         <v>11</v>
       </c>
       <c r="R41" s="5" t="str">
-        <f t="shared" ref="R41:R42" si="24">Q41&amp;" Initial Stream"</f>
+        <f t="shared" ref="R41:R42" si="25">Q41&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S41" s="5" t="str">
-        <f t="shared" ref="S41:S42" si="25">Q41</f>
+        <f t="shared" ref="S41:S42" si="26">Q41</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V41" s="5" t="s">
@@ -3219,7 +3225,7 @@
         <v>ibm</v>
       </c>
       <c r="Y41" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3228,7 +3234,7 @@
         <v>82</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="F42" s="5">
@@ -3250,11 +3256,11 @@
         <v>11</v>
       </c>
       <c r="R42" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S42" s="5" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="V42" s="5" t="s">
@@ -3269,7 +3275,7 @@
         <v>ibm</v>
       </c>
       <c r="Y42" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3278,7 +3284,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="F43" s="5">
@@ -3300,11 +3306,11 @@
         <v>11</v>
       </c>
       <c r="R43" s="5" t="str">
-        <f t="shared" ref="R43" si="26">Q43&amp;" Initial Stream"</f>
+        <f t="shared" ref="R43" si="27">Q43&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S43" s="5" t="str">
-        <f t="shared" ref="S43" si="27">Q43</f>
+        <f t="shared" ref="S43" si="28">Q43</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V43" s="5" t="s">
@@ -3319,7 +3325,7 @@
         <v>ibm</v>
       </c>
       <c r="Y43" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3328,8 +3334,11 @@
         <v>82</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="F44" s="5">
         <v>1652</v>
@@ -3339,7 +3348,7 @@
       </c>
       <c r="I44" s="8"/>
       <c r="M44" s="6" t="str">
-        <f t="shared" ref="M44:M46" si="28">"tests\results\test"&amp;C44&amp;".csv"</f>
+        <f t="shared" ref="M44:M46" si="29">"tests\results\test"&amp;C44&amp;".csv"</f>
         <v>tests\results\test141.csv</v>
       </c>
       <c r="Q44" s="5" t="s">
@@ -3363,7 +3372,7 @@
         <v>ibm</v>
       </c>
       <c r="Y44" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3372,7 +3381,7 @@
         <v>82</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="F45" s="5">
@@ -3383,7 +3392,7 @@
       </c>
       <c r="I45" s="8"/>
       <c r="M45" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>tests\results\test142.csv</v>
       </c>
       <c r="Q45" s="5" t="s">
@@ -3399,15 +3408,15 @@
         <v>12</v>
       </c>
       <c r="W45" s="5" t="str">
-        <f t="shared" ref="W45:Y46" si="29">W$2</f>
+        <f t="shared" ref="W45:X46" si="30">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X45" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>ibm</v>
       </c>
       <c r="Y45" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3416,7 +3425,7 @@
         <v>82</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="F46" s="5">
@@ -3427,7 +3436,7 @@
       </c>
       <c r="I46" s="8"/>
       <c r="M46" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>tests\results\test143.csv</v>
       </c>
       <c r="Q46" s="5" t="s">
@@ -3443,15 +3452,15 @@
         <v>12</v>
       </c>
       <c r="W46" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>ibm</v>
       </c>
       <c r="X46" s="5" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>ibm</v>
       </c>
       <c r="Y46" s="5" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="2"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3460,7 +3469,7 @@
         <v>82</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144</v>
       </c>
       <c r="F47" s="5">
@@ -3471,7 +3480,7 @@
       </c>
       <c r="I47" s="8"/>
       <c r="M47" s="6" t="str">
-        <f t="shared" ref="M47:M48" si="30">"tests\results\test"&amp;C47&amp;".csv"</f>
+        <f t="shared" ref="M47:M48" si="31">"tests\results\test"&amp;C47&amp;".csv"</f>
         <v>tests\results\test144.csv</v>
       </c>
       <c r="Q47" s="5" t="s">
@@ -3489,7 +3498,7 @@
         <v>82</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="F48" s="5">
@@ -3506,29 +3515,29 @@
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>tests\results\test145.csv</v>
       </c>
       <c r="Q48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R48" s="5" t="str">
-        <f t="shared" ref="R48" si="31">Q48&amp;" Initial Stream"</f>
+        <f t="shared" ref="R48" si="32">Q48&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S48" s="5" t="str">
-        <f t="shared" ref="S48" si="32">Q48</f>
+        <f t="shared" ref="S48" si="33">Q48</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="W48" s="5" t="str">
-        <f t="shared" ref="W48:Y52" si="33">W$2</f>
+        <f t="shared" ref="W48:X52" si="34">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X48" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="Y48" s="5" t="str">
@@ -3541,7 +3550,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="F49" s="5">
@@ -3558,29 +3567,29 @@
       </c>
       <c r="L49" s="6"/>
       <c r="M49" s="6" t="str">
-        <f t="shared" ref="M49" si="34">"tests\results\test"&amp;C49&amp;".csv"</f>
+        <f t="shared" ref="M49" si="35">"tests\results\test"&amp;C49&amp;".csv"</f>
         <v>tests\results\test146.csv</v>
       </c>
       <c r="Q49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R49" s="5" t="str">
-        <f t="shared" ref="R49" si="35">Q49&amp;" Initial Stream"</f>
+        <f t="shared" ref="R49" si="36">Q49&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S49" s="5" t="str">
-        <f t="shared" ref="S49" si="36">Q49</f>
+        <f t="shared" ref="S49" si="37">Q49</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="W49" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="X49" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="Y49" s="5" t="str">
@@ -3593,7 +3602,7 @@
         <v>82</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>147</v>
       </c>
       <c r="F50" s="5">
@@ -3610,29 +3619,29 @@
       </c>
       <c r="L50" s="6"/>
       <c r="M50" s="6" t="str">
-        <f t="shared" ref="M50" si="37">"tests\results\test"&amp;C50&amp;".csv"</f>
+        <f t="shared" ref="M50" si="38">"tests\results\test"&amp;C50&amp;".csv"</f>
         <v>tests\results\test147.csv</v>
       </c>
       <c r="Q50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R50" s="5" t="str">
-        <f t="shared" ref="R50" si="38">Q50&amp;" Initial Stream"</f>
+        <f t="shared" ref="R50" si="39">Q50&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S50" s="5" t="str">
-        <f t="shared" ref="S50" si="39">Q50</f>
+        <f t="shared" ref="S50" si="40">Q50</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="W50" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="X50" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="Y50" s="5" t="str">
@@ -3645,7 +3654,7 @@
         <v>82</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="F51" s="5">
@@ -3662,29 +3671,29 @@
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="6" t="str">
-        <f t="shared" ref="M51" si="40">"tests\results\test"&amp;C51&amp;".csv"</f>
+        <f t="shared" ref="M51" si="41">"tests\results\test"&amp;C51&amp;".csv"</f>
         <v>tests\results\test148.csv</v>
       </c>
       <c r="Q51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R51" s="5" t="str">
-        <f t="shared" ref="R51" si="41">Q51&amp;" Initial Stream"</f>
+        <f t="shared" ref="R51" si="42">Q51&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S51" s="5" t="str">
-        <f t="shared" ref="S51" si="42">Q51</f>
+        <f t="shared" ref="S51" si="43">Q51</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V51" s="5" t="s">
         <v>12</v>
       </c>
       <c r="W51" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="X51" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="Y51" s="5" t="str">
@@ -3697,7 +3706,7 @@
         <v>82</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>149</v>
       </c>
       <c r="F52" s="5">
@@ -3714,29 +3723,29 @@
       </c>
       <c r="L52" s="6"/>
       <c r="M52" s="6" t="str">
-        <f t="shared" ref="M52" si="43">"tests\results\test"&amp;C52&amp;".csv"</f>
+        <f t="shared" ref="M52" si="44">"tests\results\test"&amp;C52&amp;".csv"</f>
         <v>tests\results\test149.csv</v>
       </c>
       <c r="Q52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R52" s="5" t="str">
-        <f t="shared" ref="R52" si="44">Q52&amp;" Initial Stream"</f>
+        <f t="shared" ref="R52" si="45">Q52&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S52" s="5" t="str">
-        <f t="shared" ref="S52" si="45">Q52</f>
+        <f t="shared" ref="S52" si="46">Q52</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>12</v>
       </c>
       <c r="W52" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="X52" s="5" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>ibm</v>
       </c>
       <c r="Y52" s="5" t="str">
@@ -3770,19 +3779,19 @@
         <v>8</v>
       </c>
       <c r="M56" s="13" t="str">
-        <f t="shared" ref="M56:M57" si="46">"tests\results\test"&amp;C56&amp;".csv"</f>
+        <f t="shared" ref="M56:M57" si="47">"tests\results\test"&amp;C56&amp;".csv"</f>
         <v>tests\results\test201.csv</v>
       </c>
       <c r="W56" s="9" t="str">
-        <f t="shared" ref="W56:Y65" si="47">W$2</f>
+        <f t="shared" ref="W56:X65" si="48">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X56" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y56" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" ref="Y56:Y65" si="49">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3807,19 +3816,19 @@
         <v>212</v>
       </c>
       <c r="M57" s="13" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>tests\results\test202.csv</v>
       </c>
       <c r="W57" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X57" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y57" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3828,7 +3837,7 @@
         <v>83</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" ref="C58:C63" si="48">C57+1</f>
+        <f t="shared" ref="C58:C63" si="50">C57+1</f>
         <v>203</v>
       </c>
       <c r="E58" s="9" t="s">
@@ -3844,19 +3853,19 @@
         <v>35</v>
       </c>
       <c r="M58" s="13" t="str">
-        <f t="shared" ref="M58" si="49">"tests\results\test"&amp;C58&amp;".csv"</f>
+        <f t="shared" ref="M58" si="51">"tests\results\test"&amp;C58&amp;".csv"</f>
         <v>tests\results\test203.csv</v>
       </c>
       <c r="W58" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X58" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y58" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3865,7 +3874,7 @@
         <v>83</v>
       </c>
       <c r="C59" s="9">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>204</v>
       </c>
       <c r="E59" s="9" t="s">
@@ -3878,7 +3887,7 @@
         <v>95</v>
       </c>
       <c r="M59" s="13" t="str">
-        <f t="shared" ref="M59:M60" si="50">"tests\results\test"&amp;C59&amp;".csv"</f>
+        <f t="shared" ref="M59:M60" si="52">"tests\results\test"&amp;C59&amp;".csv"</f>
         <v>tests\results\test204.csv</v>
       </c>
       <c r="Q59" s="9" t="s">
@@ -3891,15 +3900,15 @@
         <v>79</v>
       </c>
       <c r="W59" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X59" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y59" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA59" s="9" t="s">
@@ -3911,7 +3920,7 @@
         <v>169</v>
       </c>
       <c r="C60" s="9">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>205</v>
       </c>
       <c r="E60" s="9" t="s">
@@ -3927,7 +3936,7 @@
         <v>92</v>
       </c>
       <c r="M60" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q60" s="9" t="s">
@@ -3940,15 +3949,15 @@
         <v>79</v>
       </c>
       <c r="W60" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X60" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y60" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3957,7 +3966,7 @@
         <v>169</v>
       </c>
       <c r="C61" s="9">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>206</v>
       </c>
       <c r="E61" s="9" t="s">
@@ -3986,15 +3995,15 @@
         <v>79</v>
       </c>
       <c r="W61" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X61" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y61" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4003,7 +4012,7 @@
         <v>169</v>
       </c>
       <c r="C62" s="9">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>207</v>
       </c>
       <c r="E62" s="9" t="s">
@@ -4032,15 +4041,15 @@
         <v>79</v>
       </c>
       <c r="W62" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X62" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y62" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4049,7 +4058,7 @@
         <v>169</v>
       </c>
       <c r="C63" s="9">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>208</v>
       </c>
       <c r="E63" s="9" t="s">
@@ -4078,15 +4087,15 @@
         <v>79</v>
       </c>
       <c r="W63" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X63" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y63" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4102,15 +4111,15 @@
         <v>79</v>
       </c>
       <c r="W64" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X64" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y64" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4126,15 +4135,15 @@
         <v>79</v>
       </c>
       <c r="W65" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="X65" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>ibm</v>
       </c>
       <c r="Y65" s="9" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="49"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4164,22 +4173,22 @@
         <v>8</v>
       </c>
       <c r="M69" s="11" t="str">
-        <f t="shared" ref="M69:M75" si="51">"tests\results\test"&amp;C69&amp;".csv"</f>
+        <f t="shared" ref="M69:M75" si="53">"tests\results\test"&amp;C69&amp;".csv"</f>
         <v>tests\results\test301.csv</v>
       </c>
       <c r="Q69" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W69" s="4" t="str">
-        <f t="shared" ref="W69:Y84" si="52">W$2</f>
+        <f t="shared" ref="W69:X84" si="54">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X69" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y69" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" ref="Y69:Y84" si="55">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA69" s="4" t="s">
@@ -4210,22 +4219,22 @@
         <v>8</v>
       </c>
       <c r="M70" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test302.csv</v>
       </c>
       <c r="Q70" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W70" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X70" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y70" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4234,7 +4243,7 @@
         <v>98</v>
       </c>
       <c r="C71" s="4">
-        <f t="shared" ref="C71:C80" si="53">C70+1</f>
+        <f t="shared" ref="C71:C80" si="56">C70+1</f>
         <v>303</v>
       </c>
       <c r="E71" s="4" t="s">
@@ -4253,22 +4262,22 @@
         <v>8</v>
       </c>
       <c r="M71" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test303.csv</v>
       </c>
       <c r="Q71" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W71" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X71" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y71" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4277,7 +4286,7 @@
         <v>98</v>
       </c>
       <c r="C72" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>304</v>
       </c>
       <c r="E72" s="4" t="s">
@@ -4296,22 +4305,22 @@
         <v>8</v>
       </c>
       <c r="M72" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test304.csv</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W72" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X72" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y72" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4320,7 +4329,7 @@
         <v>98</v>
       </c>
       <c r="C73" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>305</v>
       </c>
       <c r="E73" s="4" t="s">
@@ -4339,22 +4348,22 @@
         <v>163</v>
       </c>
       <c r="M73" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test305.csv</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W73" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X73" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y73" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4363,7 +4372,7 @@
         <v>98</v>
       </c>
       <c r="C74" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>306</v>
       </c>
       <c r="E74" s="4" t="s">
@@ -4382,22 +4391,22 @@
         <v>8</v>
       </c>
       <c r="M74" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test306.csv</v>
       </c>
       <c r="Q74" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W74" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X74" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y74" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4406,7 +4415,7 @@
         <v>98</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>307</v>
       </c>
       <c r="E75" s="4" t="s">
@@ -4425,22 +4434,22 @@
         <v>8</v>
       </c>
       <c r="M75" s="11" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>tests\results\test307.csv</v>
       </c>
       <c r="Q75" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W75" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X75" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y75" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4449,7 +4458,7 @@
         <v>98</v>
       </c>
       <c r="C76" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>308</v>
       </c>
       <c r="E76" s="4" t="s">
@@ -4465,7 +4474,7 @@
         <v>8</v>
       </c>
       <c r="M76" s="11" t="str">
-        <f t="shared" ref="M76:M80" si="54">"tests\results\test"&amp;C76&amp;".csv"</f>
+        <f t="shared" ref="M76:M80" si="57">"tests\results\test"&amp;C76&amp;".csv"</f>
         <v>tests\results\test308.csv</v>
       </c>
       <c r="N76" s="4" t="s">
@@ -4475,15 +4484,15 @@
         <v>87</v>
       </c>
       <c r="W76" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X76" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y76" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4492,7 +4501,7 @@
         <v>98</v>
       </c>
       <c r="C77" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>309</v>
       </c>
       <c r="E77" s="4" t="s">
@@ -4508,7 +4517,7 @@
         <v>8</v>
       </c>
       <c r="M77" s="11" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>tests\results\test309.csv</v>
       </c>
       <c r="P77" s="4" t="s">
@@ -4518,15 +4527,15 @@
         <v>87</v>
       </c>
       <c r="W77" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X77" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y77" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4535,7 +4544,7 @@
         <v>98</v>
       </c>
       <c r="C78" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>310</v>
       </c>
       <c r="E78" s="4" t="s">
@@ -4554,22 +4563,22 @@
         <v>8</v>
       </c>
       <c r="M78" s="11" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>tests\results\test310.csv</v>
       </c>
       <c r="Q78" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W78" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X78" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y78" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4578,7 +4587,7 @@
         <v>98</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>311</v>
       </c>
       <c r="E79" s="4" t="s">
@@ -4594,22 +4603,22 @@
         <v>205</v>
       </c>
       <c r="M79" s="11" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>tests\results\test311.csv</v>
       </c>
       <c r="Q79" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W79" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X79" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y79" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4618,7 +4627,7 @@
         <v>98</v>
       </c>
       <c r="C80" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>312</v>
       </c>
       <c r="E80" s="4" t="s">
@@ -4634,7 +4643,7 @@
         <v>8</v>
       </c>
       <c r="M80" s="11" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>tests\results\test312.csv</v>
       </c>
       <c r="N80" s="4" t="s">
@@ -4644,15 +4653,15 @@
         <v>87</v>
       </c>
       <c r="W80" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X80" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y80" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
       <c r="AA80" s="4" t="s">
@@ -4665,15 +4674,15 @@
         <v>87</v>
       </c>
       <c r="W81" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X81" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y81" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4683,15 +4692,15 @@
         <v>87</v>
       </c>
       <c r="W82" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X82" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y82" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4701,15 +4710,15 @@
         <v>87</v>
       </c>
       <c r="W83" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X83" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y83" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4719,15 +4728,15 @@
         <v>87</v>
       </c>
       <c r="W84" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="X84" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>ibm</v>
       </c>
       <c r="Y84" s="4" t="str">
-        <f>Y$2</f>
+        <f t="shared" si="55"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4762,15 +4771,15 @@
         <v>8</v>
       </c>
       <c r="M88" s="10" t="str">
-        <f t="shared" ref="M88:M92" si="55">"tests\results\test"&amp;C88&amp;".csv"</f>
+        <f t="shared" ref="M88:M92" si="58">"tests\results\test"&amp;C88&amp;".csv"</f>
         <v>tests\results\test401.csv</v>
       </c>
       <c r="W88" s="3" t="str">
-        <f t="shared" ref="W88:Y92" si="56">W$2</f>
+        <f t="shared" ref="W88:X92" si="59">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X88" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="Y88" s="3" t="str">
@@ -4802,15 +4811,15 @@
         <v>8</v>
       </c>
       <c r="M89" s="10" t="str">
-        <f t="shared" ref="M89" si="57">"tests\results\test"&amp;C89&amp;".csv"</f>
+        <f t="shared" ref="M89" si="60">"tests\results\test"&amp;C89&amp;".csv"</f>
         <v>tests\results\test402.csv</v>
       </c>
       <c r="W89" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="X89" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="Y89" s="3" t="str">
@@ -4823,7 +4832,7 @@
         <v>85</v>
       </c>
       <c r="C90" s="3">
-        <f t="shared" ref="C90:C92" si="58">C89+1</f>
+        <f t="shared" ref="C90:C92" si="61">C89+1</f>
         <v>403</v>
       </c>
       <c r="E90" s="3" t="s">
@@ -4842,18 +4851,18 @@
         <v>8</v>
       </c>
       <c r="M90" s="10" t="str">
-        <f t="shared" ref="M90" si="59">"tests\results\test"&amp;C90&amp;".csv"</f>
+        <f t="shared" ref="M90" si="62">"tests\results\test"&amp;C90&amp;".csv"</f>
         <v>tests\results\test403.csv</v>
       </c>
       <c r="Q90" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W90" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="X90" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="Y90" s="3" t="str">
@@ -4869,7 +4878,7 @@
         <v>85</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>404</v>
       </c>
       <c r="E91" s="3" t="s">
@@ -4888,7 +4897,7 @@
         <v>8</v>
       </c>
       <c r="M91" s="10" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>tests\results\test404.csv</v>
       </c>
       <c r="Q91" s="3" t="s">
@@ -4901,11 +4910,11 @@
         <v>181</v>
       </c>
       <c r="W91" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="X91" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="Y91" s="3" t="str">
@@ -4918,7 +4927,7 @@
         <v>97</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>405</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -4940,18 +4949,18 @@
         <v>8</v>
       </c>
       <c r="M92" s="10" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>tests\results\test405.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>89</v>
       </c>
       <c r="W92" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="X92" s="3" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>ibm</v>
       </c>
       <c r="Y92" s="3" t="str">
@@ -5001,11 +5010,11 @@
         <v>11</v>
       </c>
       <c r="R98" s="14" t="str">
-        <f t="shared" ref="R98:R107" si="60">Q98&amp;" Initial Stream"</f>
+        <f t="shared" ref="R98:R107" si="63">Q98&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S98" s="14" t="str">
-        <f t="shared" ref="S98:S106" si="61">Q98</f>
+        <f t="shared" ref="S98:S106" si="64">Q98</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="W98" s="5" t="str">
@@ -5050,11 +5059,11 @@
         <v>11</v>
       </c>
       <c r="R99" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S99" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W99" s="14" t="s">
@@ -5075,7 +5084,7 @@
         <v>141</v>
       </c>
       <c r="C100" s="14">
-        <f t="shared" ref="C100:C107" si="62">C99+1</f>
+        <f t="shared" ref="C100:C107" si="65">C99+1</f>
         <v>1003</v>
       </c>
       <c r="D100" s="14" t="s">
@@ -5096,11 +5105,11 @@
         <v>11</v>
       </c>
       <c r="R100" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S100" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W100" s="14" t="s">
@@ -5124,7 +5133,7 @@
         <v>141</v>
       </c>
       <c r="C101" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1004</v>
       </c>
       <c r="G101" s="14" t="s">
@@ -5142,11 +5151,11 @@
         <v>11</v>
       </c>
       <c r="R101" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S101" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
@@ -5167,7 +5176,7 @@
         <v>141</v>
       </c>
       <c r="C102" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1005</v>
       </c>
       <c r="D102" s="14" t="s">
@@ -5188,11 +5197,11 @@
         <v>11</v>
       </c>
       <c r="R102" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S102" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
@@ -5213,7 +5222,7 @@
         <v>141</v>
       </c>
       <c r="C103" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1006</v>
       </c>
       <c r="G103" s="14" t="s">
@@ -5231,11 +5240,11 @@
         <v>11</v>
       </c>
       <c r="R103" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S103" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W103" s="5" t="str">
@@ -5262,7 +5271,7 @@
         <v>141</v>
       </c>
       <c r="C104" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1007</v>
       </c>
       <c r="G104" s="14" t="s">
@@ -5280,11 +5289,11 @@
         <v>11</v>
       </c>
       <c r="R104" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S104" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W104" s="14" t="s">
@@ -5308,7 +5317,7 @@
         <v>141</v>
       </c>
       <c r="C105" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1008</v>
       </c>
       <c r="D105" s="14" t="s">
@@ -5329,11 +5338,11 @@
         <v>11</v>
       </c>
       <c r="R105" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S105" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W105" s="14" t="s">
@@ -5357,7 +5366,7 @@
         <v>141</v>
       </c>
       <c r="C106" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1009</v>
       </c>
       <c r="D106" s="14" t="s">
@@ -5378,11 +5387,11 @@
         <v>11</v>
       </c>
       <c r="R106" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S106" s="14" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
@@ -5403,7 +5412,7 @@
         <v>141</v>
       </c>
       <c r="C107" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1010</v>
       </c>
       <c r="G107" s="14" t="s">
@@ -5421,11 +5430,11 @@
         <v>11</v>
       </c>
       <c r="R107" s="14" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S107" s="14" t="str">
-        <f t="shared" ref="S107" si="63">Q107</f>
+        <f t="shared" ref="S107" si="66">Q107</f>
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">

</xml_diff>

<commit_message>
added ccm to represt (unfinished), fixed problem finding config
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests.xlsx
+++ b/elmclient/tests/tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013CD760-4CE2-49D6-B1A2-F306A947FD2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B91C7E8-6AC6-4FBB-AC27-82D042F75E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="-20760" windowWidth="29655" windowHeight="16050" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="-24480" yWindow="-20895" windowWidth="29655" windowHeight="16050" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed problem querying non-default component
</commit_message>
<xml_diff>
--- a/elmclient/tests/tests.xlsx
+++ b/elmclient/tests/tests.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B91C7E8-6AC6-4FBB-AC27-82D042F75E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0AD490-B3C4-4A64-9C44-B7E2F3F47933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24480" yWindow="-20895" windowWidth="29655" windowHeight="16050" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
+    <workbookView xWindow="14160" yWindow="-21090" windowWidth="32565" windowHeight="17865" xr2:uid="{E12FDD20-F1C7-4695-B929-60D3CA2A8B69}"/>
   </bookViews>
   <sheets>
     <sheet name="rmqueries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="229">
   <si>
     <t>oslc_rm:uses</t>
   </si>
@@ -709,6 +709,12 @@
   </si>
   <si>
     <t>rm,gc</t>
+  </si>
+  <si>
+    <t>All artifacts created by fred</t>
+  </si>
+  <si>
+    <t># FAILS!</t>
   </si>
 </sst>
 </file>
@@ -1155,11 +1161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CC5532-4E98-4C99-BC3C-1388DFEBC8F1}">
-  <dimension ref="A1:AH109"/>
+  <dimension ref="A1:AH110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1455,7 @@
         <v>82</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" ref="C6:C52" si="3">C5+1</f>
+        <f t="shared" ref="C6:C53" si="3">C5+1</f>
         <v>103</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -2848,7 +2854,7 @@
         <v>131</v>
       </c>
       <c r="F34" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>111</v>
@@ -2899,7 +2905,7 @@
         <v>132</v>
       </c>
       <c r="F35" s="5">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>115</v>
@@ -3533,7 +3539,7 @@
         <v>12</v>
       </c>
       <c r="W48" s="5" t="str">
-        <f t="shared" ref="W48:X52" si="34">W$2</f>
+        <f t="shared" ref="W48:X53" si="34">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X48" s="5" t="str">
@@ -3753,46 +3759,65 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="5">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6" t="str">
+        <f t="shared" ref="M53" si="47">"tests\results\test"&amp;C53&amp;".csv"</f>
+        <v>tests\results\test150.csv</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R53" s="5" t="str">
+        <f t="shared" ref="R53" si="48">Q53&amp;" Initial Stream"</f>
+        <v>rm_optout_p1 Initial Stream</v>
+      </c>
+      <c r="S53" s="5" t="str">
+        <f t="shared" ref="S53" si="49">Q53</f>
+        <v>rm_optout_p1</v>
+      </c>
+      <c r="V53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W53" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>ibm</v>
+      </c>
+      <c r="X53" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y53" s="5" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="9">
-        <v>201</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F56" s="9">
-        <v>15</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="J56" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M56" s="13" t="str">
-        <f t="shared" ref="M56:M57" si="47">"tests\results\test"&amp;C56&amp;".csv"</f>
-        <v>tests\results\test201.csv</v>
-      </c>
-      <c r="W56" s="9" t="str">
-        <f t="shared" ref="W56:X65" si="48">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X56" s="9" t="str">
-        <f t="shared" si="48"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y56" s="9" t="str">
-        <f t="shared" ref="Y56:Y65" si="49">Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3800,35 +3825,34 @@
         <v>83</v>
       </c>
       <c r="C57" s="9">
-        <f>C56+1</f>
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F57" s="9">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="I57" s="9" t="s">
-        <v>212</v>
+        <v>182</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="M57" s="13" t="str">
-        <f t="shared" si="47"/>
-        <v>tests\results\test202.csv</v>
+        <f t="shared" ref="M57:M58" si="50">"tests\results\test"&amp;C57&amp;".csv"</f>
+        <v>tests\results\test201.csv</v>
       </c>
       <c r="W57" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="W57:X66" si="51">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X57" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y57" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="Y57:Y66" si="52">Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3837,35 +3861,35 @@
         <v>83</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" ref="C58:C63" si="50">C57+1</f>
-        <v>203</v>
+        <f>C57+1</f>
+        <v>202</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F58" s="9">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>35</v>
+        <v>224</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="M58" s="13" t="str">
-        <f t="shared" ref="M58" si="51">"tests\results\test"&amp;C58&amp;".csv"</f>
-        <v>tests\results\test203.csv</v>
+        <f t="shared" si="50"/>
+        <v>tests\results\test202.csv</v>
       </c>
       <c r="W58" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X58" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y58" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -3874,70 +3898,58 @@
         <v>83</v>
       </c>
       <c r="C59" s="9">
-        <f t="shared" si="50"/>
-        <v>204</v>
+        <f t="shared" ref="C59:C64" si="53">C58+1</f>
+        <v>203</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F59" s="9">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>95</v>
+        <v>183</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="M59" s="13" t="str">
-        <f t="shared" ref="M59:M60" si="52">"tests\results\test"&amp;C59&amp;".csv"</f>
-        <v>tests\results\test204.csv</v>
-      </c>
-      <c r="Q59" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="R59" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="S59" s="9" t="s">
-        <v>79</v>
+        <f t="shared" ref="M59" si="54">"tests\results\test"&amp;C59&amp;".csv"</f>
+        <v>tests\results\test203.csv</v>
       </c>
       <c r="W59" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X59" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y59" s="9" t="str">
-        <f t="shared" si="49"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA59" s="9" t="s">
-        <v>125</v>
+        <f t="shared" si="52"/>
+        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="60" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="C60" s="9">
-        <f t="shared" si="50"/>
-        <v>205</v>
+        <f t="shared" si="53"/>
+        <v>204</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F60" s="9">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M60" s="13" t="str">
-        <f t="shared" si="52"/>
-        <v>tests\results\test205.csv</v>
+        <f t="shared" ref="M60:M61" si="55">"tests\results\test"&amp;C60&amp;".csv"</f>
+        <v>tests\results\test204.csv</v>
       </c>
       <c r="Q60" s="9" t="s">
         <v>78</v>
@@ -3949,16 +3961,19 @@
         <v>79</v>
       </c>
       <c r="W60" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X60" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y60" s="9" t="str">
-        <f t="shared" si="49"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" si="52"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA60" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3966,23 +3981,23 @@
         <v>169</v>
       </c>
       <c r="C61" s="9">
-        <f t="shared" si="50"/>
-        <v>206</v>
+        <f t="shared" si="53"/>
+        <v>205</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F61" s="9">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="I61" s="9" t="s">
-        <v>170</v>
+        <v>96</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="M61" s="13" t="str">
-        <f>"tests\results\test"&amp;C60&amp;".csv"</f>
+        <f t="shared" si="55"/>
         <v>tests\results\test205.csv</v>
       </c>
       <c r="Q61" s="9" t="s">
@@ -3995,15 +4010,15 @@
         <v>79</v>
       </c>
       <c r="W61" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X61" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y61" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4012,24 +4027,24 @@
         <v>169</v>
       </c>
       <c r="C62" s="9">
-        <f t="shared" si="50"/>
-        <v>207</v>
+        <f t="shared" si="53"/>
+        <v>206</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F62" s="9">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="M62" s="13" t="str">
         <f>"tests\results\test"&amp;C61&amp;".csv"</f>
-        <v>tests\results\test206.csv</v>
-      </c>
-      <c r="N62" s="9" t="s">
-        <v>173</v>
+        <v>tests\results\test205.csv</v>
       </c>
       <c r="Q62" s="9" t="s">
         <v>78</v>
@@ -4041,15 +4056,15 @@
         <v>79</v>
       </c>
       <c r="W62" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X62" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y62" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4058,23 +4073,23 @@
         <v>169</v>
       </c>
       <c r="C63" s="9">
-        <f t="shared" si="50"/>
-        <v>208</v>
+        <f t="shared" si="53"/>
+        <v>207</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>72</v>
       </c>
       <c r="F63" s="9">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M63" s="13" t="str">
         <f>"tests\results\test"&amp;C62&amp;".csv"</f>
-        <v>tests\results\test207.csv</v>
-      </c>
-      <c r="P63" s="9" t="s">
+        <v>tests\results\test206.csv</v>
+      </c>
+      <c r="N63" s="9" t="s">
         <v>173</v>
       </c>
       <c r="Q63" s="9" t="s">
@@ -4087,20 +4102,42 @@
         <v>79</v>
       </c>
       <c r="W63" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X63" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y63" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="64" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M64" s="13"/>
+      <c r="B64" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" s="9">
+        <f t="shared" si="53"/>
+        <v>208</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F64" s="9">
+        <v>8</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="M64" s="13" t="str">
+        <f>"tests\results\test"&amp;C63&amp;".csv"</f>
+        <v>tests\results\test207.csv</v>
+      </c>
+      <c r="P64" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="Q64" s="9" t="s">
         <v>78</v>
       </c>
@@ -4111,15 +4148,15 @@
         <v>79</v>
       </c>
       <c r="W64" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X64" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y64" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4135,107 +4172,88 @@
         <v>79</v>
       </c>
       <c r="W65" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="X65" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>ibm</v>
       </c>
       <c r="Y65" s="9" t="str">
-        <f t="shared" si="49"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-    </row>
-    <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+        <f t="shared" si="52"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M66" s="13"/>
+      <c r="Q66" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S66" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="W66" s="9" t="str">
+        <f t="shared" si="51"/>
+        <v>ibm</v>
+      </c>
+      <c r="X66" s="9" t="str">
+        <f t="shared" si="51"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y66" s="9" t="str">
+        <f t="shared" si="52"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="69" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C69" s="4">
-        <v>301</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F69" s="4">
-        <v>89</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M69" s="11" t="str">
-        <f t="shared" ref="M69:M75" si="53">"tests\results\test"&amp;C69&amp;".csv"</f>
-        <v>tests\results\test301.csv</v>
-      </c>
-      <c r="Q69" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="W69" s="4" t="str">
-        <f t="shared" ref="W69:X84" si="54">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X69" s="4" t="str">
-        <f t="shared" si="54"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y69" s="4" t="str">
-        <f t="shared" ref="Y69:Y84" si="55">Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA69" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C70" s="4">
-        <f>C69+1</f>
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F70" s="4">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M70" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test302.csv</v>
+        <f t="shared" ref="M70:M76" si="56">"tests\results\test"&amp;C70&amp;".csv"</f>
+        <v>tests\results\test301.csv</v>
       </c>
       <c r="Q70" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W70" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="W70:X85" si="57">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X70" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y70" s="4" t="str">
-        <f t="shared" si="55"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" ref="Y70:Y85" si="58">Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA70" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4243,41 +4261,41 @@
         <v>98</v>
       </c>
       <c r="C71" s="4">
-        <f t="shared" ref="C71:C80" si="56">C70+1</f>
-        <v>303</v>
+        <f>C70+1</f>
+        <v>302</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F71" s="4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>160</v>
+        <v>99</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M71" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test303.csv</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test302.csv</v>
       </c>
       <c r="Q71" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W71" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X71" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y71" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4286,41 +4304,41 @@
         <v>98</v>
       </c>
       <c r="C72" s="4">
-        <f t="shared" si="56"/>
-        <v>304</v>
+        <f t="shared" ref="C72:C81" si="59">C71+1</f>
+        <v>303</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F72" s="4">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M72" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test304.csv</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test303.csv</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W72" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X72" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y72" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4329,41 +4347,41 @@
         <v>98</v>
       </c>
       <c r="C73" s="4">
-        <f t="shared" si="56"/>
-        <v>305</v>
+        <f t="shared" si="59"/>
+        <v>304</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F73" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K73" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="M73" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test305.csv</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test304.csv</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W73" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X73" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y73" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4372,41 +4390,41 @@
         <v>98</v>
       </c>
       <c r="C74" s="4">
-        <f t="shared" si="56"/>
-        <v>306</v>
+        <f t="shared" si="59"/>
+        <v>305</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F74" s="4">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="K74" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="M74" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test306.csv</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test305.csv</v>
       </c>
       <c r="Q74" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W74" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X74" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y74" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4415,41 +4433,41 @@
         <v>98</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" si="56"/>
-        <v>307</v>
+        <f t="shared" si="59"/>
+        <v>306</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F75" s="4">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M75" s="11" t="str">
-        <f t="shared" si="53"/>
-        <v>tests\results\test307.csv</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test306.csv</v>
       </c>
       <c r="Q75" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W75" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X75" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y75" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4458,41 +4476,41 @@
         <v>98</v>
       </c>
       <c r="C76" s="4">
-        <f t="shared" si="56"/>
-        <v>308</v>
+        <f t="shared" si="59"/>
+        <v>307</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F76" s="4">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M76" s="11" t="str">
-        <f t="shared" ref="M76:M80" si="57">"tests\results\test"&amp;C76&amp;".csv"</f>
-        <v>tests\results\test308.csv</v>
-      </c>
-      <c r="N76" s="4" t="s">
-        <v>175</v>
+        <f t="shared" si="56"/>
+        <v>tests\results\test307.csv</v>
       </c>
       <c r="Q76" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W76" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X76" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y76" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4501,41 +4519,41 @@
         <v>98</v>
       </c>
       <c r="C77" s="4">
-        <f t="shared" si="56"/>
-        <v>309</v>
+        <f t="shared" si="59"/>
+        <v>308</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F77" s="4">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M77" s="11" t="str">
-        <f t="shared" si="57"/>
-        <v>tests\results\test309.csv</v>
-      </c>
-      <c r="P77" s="4" t="s">
+        <f t="shared" ref="M77:M81" si="60">"tests\results\test"&amp;C77&amp;".csv"</f>
+        <v>tests\results\test308.csv</v>
+      </c>
+      <c r="N77" s="4" t="s">
         <v>175</v>
       </c>
       <c r="Q77" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W77" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X77" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y77" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4544,41 +4562,41 @@
         <v>98</v>
       </c>
       <c r="C78" s="4">
-        <f t="shared" si="56"/>
-        <v>310</v>
+        <f t="shared" si="59"/>
+        <v>309</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F78" s="4">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="I78" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M78" s="11" t="str">
-        <f t="shared" si="57"/>
-        <v>tests\results\test310.csv</v>
+        <f t="shared" si="60"/>
+        <v>tests\results\test309.csv</v>
+      </c>
+      <c r="P78" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="Q78" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W78" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X78" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y78" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4587,38 +4605,41 @@
         <v>98</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="56"/>
-        <v>311</v>
+        <f t="shared" si="59"/>
+        <v>310</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F79" s="4">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>205</v>
+        <v>178</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="M79" s="11" t="str">
-        <f t="shared" si="57"/>
-        <v>tests\results\test311.csv</v>
+        <f t="shared" si="60"/>
+        <v>tests\results\test310.csv</v>
       </c>
       <c r="Q79" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W79" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X79" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y79" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4627,63 +4648,85 @@
         <v>98</v>
       </c>
       <c r="C80" s="4">
-        <f t="shared" si="56"/>
-        <v>312</v>
+        <f t="shared" si="59"/>
+        <v>311</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F80" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>8</v>
+        <v>206</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="M80" s="11" t="str">
-        <f t="shared" si="57"/>
-        <v>tests\results\test312.csv</v>
-      </c>
-      <c r="N80" s="4" t="s">
-        <v>191</v>
+        <f t="shared" si="60"/>
+        <v>tests\results\test311.csv</v>
       </c>
       <c r="Q80" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W80" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X80" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y80" s="4" t="str">
-        <f t="shared" si="55"/>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA80" s="4" t="s">
-        <v>126</v>
+        <f t="shared" si="58"/>
+        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="81" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M81" s="11"/>
+      <c r="B81" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="4">
+        <f t="shared" si="59"/>
+        <v>312</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M81" s="11" t="str">
+        <f t="shared" si="60"/>
+        <v>tests\results\test312.csv</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="Q81" s="4" t="s">
         <v>87</v>
       </c>
       <c r="W81" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X81" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y81" s="4" t="str">
-        <f t="shared" si="55"/>
-        <v>https://jazz.ibm.com:9443</v>
+        <f t="shared" si="58"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AA81" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4692,15 +4735,15 @@
         <v>87</v>
       </c>
       <c r="W82" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X82" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y82" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4710,15 +4753,15 @@
         <v>87</v>
       </c>
       <c r="W83" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X83" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y83" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
@@ -4728,63 +4771,42 @@
         <v>87</v>
       </c>
       <c r="W84" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="X84" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>ibm</v>
       </c>
       <c r="Y84" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="85" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="M85" s="11"/>
-    </row>
-    <row r="87" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="Q85" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W85" s="4" t="str">
+        <f t="shared" si="57"/>
+        <v>ibm</v>
+      </c>
+      <c r="X85" s="4" t="str">
+        <f t="shared" si="57"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y85" s="4" t="str">
+        <f t="shared" si="58"/>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M86" s="11"/>
+    </row>
+    <row r="88" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" s="3">
-        <v>401</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F88" s="3">
-        <v>26</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M88" s="10" t="str">
-        <f t="shared" ref="M88:M92" si="58">"tests\results\test"&amp;C88&amp;".csv"</f>
-        <v>tests\results\test401.csv</v>
-      </c>
-      <c r="W88" s="3" t="str">
-        <f t="shared" ref="W88:X92" si="59">W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X88" s="3" t="str">
-        <f t="shared" si="59"/>
-        <v>ibm</v>
-      </c>
-      <c r="Y88" s="3" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
     <row r="89" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4792,34 +4814,33 @@
         <v>85</v>
       </c>
       <c r="C89" s="3">
-        <f>C88+1</f>
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F89" s="3">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J89" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M89" s="10" t="str">
-        <f t="shared" ref="M89" si="60">"tests\results\test"&amp;C89&amp;".csv"</f>
-        <v>tests\results\test402.csv</v>
+        <f t="shared" ref="M89:M93" si="61">"tests\results\test"&amp;C89&amp;".csv"</f>
+        <v>tests\results\test401.csv</v>
       </c>
       <c r="W89" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" ref="W89:X93" si="62">W$2</f>
         <v>ibm</v>
       </c>
       <c r="X89" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="Y89" s="3" t="str">
@@ -4832,17 +4853,17 @@
         <v>85</v>
       </c>
       <c r="C90" s="3">
-        <f t="shared" ref="C90:C92" si="61">C89+1</f>
-        <v>403</v>
+        <f>C89+1</f>
+        <v>402</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F90" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>35</v>
@@ -4851,26 +4872,20 @@
         <v>8</v>
       </c>
       <c r="M90" s="10" t="str">
-        <f t="shared" ref="M90" si="62">"tests\results\test"&amp;C90&amp;".csv"</f>
-        <v>tests\results\test403.csv</v>
-      </c>
-      <c r="Q90" s="3" t="s">
-        <v>89</v>
+        <f t="shared" ref="M90" si="63">"tests\results\test"&amp;C90&amp;".csv"</f>
+        <v>tests\results\test402.csv</v>
       </c>
       <c r="W90" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="X90" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="Y90" s="3" t="str">
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AA90" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4878,89 +4893,89 @@
         <v>85</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" si="61"/>
-        <v>404</v>
+        <f t="shared" ref="C91:C93" si="64">C90+1</f>
+        <v>403</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F91" s="3">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M91" s="10" t="str">
-        <f t="shared" si="58"/>
-        <v>tests\results\test404.csv</v>
+        <f t="shared" ref="M91" si="65">"tests\results\test"&amp;C91&amp;".csv"</f>
+        <v>tests\results\test403.csv</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="R91" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="S91" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="W91" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="X91" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="Y91" s="3" t="str">
         <f>Y$2</f>
         <v>https://jazz.ibm.com:9443</v>
       </c>
+      <c r="AA91" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="92" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="61"/>
-        <v>405</v>
+        <f t="shared" si="64"/>
+        <v>404</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F92" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I92" s="10" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M92" s="10" t="str">
-        <f t="shared" si="58"/>
-        <v>tests\results\test405.csv</v>
+        <f t="shared" si="61"/>
+        <v>tests\results\test404.csv</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="R92" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="W92" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="X92" s="3" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>ibm</v>
       </c>
       <c r="Y92" s="3" t="str">
@@ -4968,35 +4983,61 @@
         <v>https://jazz.ibm.com:9443</v>
       </c>
     </row>
-    <row r="93" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="64"/>
+        <v>405</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F93" s="3">
+        <v>1</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M93" s="10" t="str">
+        <f t="shared" si="61"/>
+        <v>tests\results\test405.csv</v>
+      </c>
+      <c r="Q93" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W93" s="3" t="str">
+        <f t="shared" si="62"/>
+        <v>ibm</v>
+      </c>
+      <c r="X93" s="3" t="str">
+        <f t="shared" si="62"/>
+        <v>ibm</v>
+      </c>
+      <c r="Y93" s="3" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+    </row>
     <row r="94" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
+    <row r="96" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="G97" s="14" t="s">
+      <c r="G98" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="I97" s="15"/>
-      <c r="J97" s="15"/>
-      <c r="K97" s="15"/>
-      <c r="L97" s="15"/>
-      <c r="M97" s="15"/>
-      <c r="N97" s="15"/>
-      <c r="O97" s="15"/>
-      <c r="P97" s="15"/>
-      <c r="Y97" s="16"/>
-    </row>
-    <row r="98" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C98" s="14">
-        <v>1001</v>
-      </c>
-      <c r="G98" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="I98" s="15"/>
       <c r="J98" s="15"/>
@@ -5006,46 +5047,17 @@
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
       <c r="P98" s="15"/>
-      <c r="Q98" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="R98" s="14" t="str">
-        <f t="shared" ref="R98:R107" si="63">Q98&amp;" Initial Stream"</f>
-        <v>rm_optout_p1 Initial Stream</v>
-      </c>
-      <c r="S98" s="14" t="str">
-        <f t="shared" ref="S98:S106" si="64">Q98</f>
-        <v>rm_optout_p1</v>
-      </c>
-      <c r="W98" s="5" t="str">
-        <f>W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X98" s="5" t="str">
-        <f>X$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="Y98" s="5" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AB98" s="14" t="s">
-        <v>142</v>
-      </c>
+      <c r="Y98" s="16"/>
     </row>
     <row r="99" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C99" s="14">
-        <f>C98+1</f>
-        <v>1002</v>
-      </c>
-      <c r="F99" s="14">
-        <v>738</v>
+        <v>1001</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
@@ -5059,23 +5071,26 @@
         <v>11</v>
       </c>
       <c r="R99" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" ref="R99:R108" si="66">Q99&amp;" Initial Stream"</f>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S99" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" ref="S99:S107" si="67">Q99</f>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W99" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="X99" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y99" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC99" s="14" t="s">
+      <c r="W99" s="5" t="str">
+        <f>W$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="X99" s="5" t="str">
+        <f>X$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="Y99" s="5" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AB99" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5084,14 +5099,14 @@
         <v>141</v>
       </c>
       <c r="C100" s="14">
-        <f t="shared" ref="C100:C107" si="65">C99+1</f>
-        <v>1003</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>143</v>
+        <f>C99+1</f>
+        <v>1002</v>
+      </c>
+      <c r="F100" s="14">
+        <v>738</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
@@ -5105,11 +5120,11 @@
         <v>11</v>
       </c>
       <c r="R100" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S100" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W100" s="14" t="s">
@@ -5123,9 +5138,6 @@
       </c>
       <c r="AC100" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="AE100" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5133,11 +5145,14 @@
         <v>141</v>
       </c>
       <c r="C101" s="14">
-        <f t="shared" si="65"/>
-        <v>1004</v>
+        <f t="shared" ref="C101:C108" si="68">C100+1</f>
+        <v>1003</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
@@ -5151,11 +5166,11 @@
         <v>11</v>
       </c>
       <c r="R101" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S101" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W101" s="14" t="s">
@@ -5167,8 +5182,11 @@
       <c r="Y101" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AD101" s="14" t="s">
+      <c r="AC101" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="AE101" s="14" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5176,14 +5194,11 @@
         <v>141</v>
       </c>
       <c r="C102" s="14">
-        <f t="shared" si="65"/>
-        <v>1005</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>143</v>
+        <f t="shared" si="68"/>
+        <v>1004</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
@@ -5197,11 +5212,11 @@
         <v>11</v>
       </c>
       <c r="R102" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S102" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W102" s="14" t="s">
@@ -5213,7 +5228,7 @@
       <c r="Y102" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AC102" s="14" t="s">
+      <c r="AD102" s="14" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5222,11 +5237,14 @@
         <v>141</v>
       </c>
       <c r="C103" s="14">
-        <f t="shared" si="65"/>
-        <v>1006</v>
+        <f t="shared" si="68"/>
+        <v>1005</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I103" s="15"/>
       <c r="J103" s="15"/>
@@ -5240,30 +5258,24 @@
         <v>11</v>
       </c>
       <c r="R103" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S103" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W103" s="5" t="str">
-        <f>W$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="X103" s="5" t="str">
-        <f>X$2</f>
-        <v>ibm</v>
-      </c>
-      <c r="Y103" s="5" t="str">
-        <f>Y$2</f>
-        <v>https://jazz.ibm.com:9443</v>
-      </c>
-      <c r="AB103" s="14" t="s">
+      <c r="W103" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X103" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y103" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC103" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="AE103" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5271,11 +5283,11 @@
         <v>141</v>
       </c>
       <c r="C104" s="14">
-        <f t="shared" si="65"/>
-        <v>1007</v>
+        <f t="shared" si="68"/>
+        <v>1006</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I104" s="15"/>
       <c r="J104" s="15"/>
@@ -5289,23 +5301,26 @@
         <v>11</v>
       </c>
       <c r="R104" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S104" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
-      <c r="W104" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="X104" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y104" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC104" s="14" t="s">
+      <c r="W104" s="5" t="str">
+        <f>W$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="X104" s="5" t="str">
+        <f>X$2</f>
+        <v>ibm</v>
+      </c>
+      <c r="Y104" s="5" t="str">
+        <f>Y$2</f>
+        <v>https://jazz.ibm.com:9443</v>
+      </c>
+      <c r="AB104" s="14" t="s">
         <v>142</v>
       </c>
       <c r="AE104" s="14" t="s">
@@ -5317,14 +5332,11 @@
         <v>141</v>
       </c>
       <c r="C105" s="14">
-        <f t="shared" si="65"/>
-        <v>1008</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>143</v>
+        <f t="shared" si="68"/>
+        <v>1007</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
@@ -5338,11 +5350,11 @@
         <v>11</v>
       </c>
       <c r="R105" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S105" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W105" s="14" t="s">
@@ -5358,7 +5370,7 @@
         <v>142</v>
       </c>
       <c r="AE105" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5366,14 +5378,14 @@
         <v>141</v>
       </c>
       <c r="C106" s="14">
-        <f t="shared" si="65"/>
-        <v>1009</v>
+        <f t="shared" si="68"/>
+        <v>1008</v>
       </c>
       <c r="D106" s="14" t="s">
         <v>143</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
@@ -5387,11 +5399,11 @@
         <v>11</v>
       </c>
       <c r="R106" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S106" s="14" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W106" s="14" t="s">
@@ -5405,6 +5417,9 @@
       </c>
       <c r="AC106" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="AE106" s="14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5412,11 +5427,14 @@
         <v>141</v>
       </c>
       <c r="C107" s="14">
-        <f t="shared" si="65"/>
-        <v>1010</v>
+        <f t="shared" si="68"/>
+        <v>1009</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -5430,11 +5448,11 @@
         <v>11</v>
       </c>
       <c r="R107" s="14" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>rm_optout_p1 Initial Stream</v>
       </c>
       <c r="S107" s="14" t="str">
-        <f t="shared" ref="S107" si="66">Q107</f>
+        <f t="shared" si="67"/>
         <v>rm_optout_p1</v>
       </c>
       <c r="W107" s="14" t="s">
@@ -5446,11 +5464,21 @@
       <c r="Y107" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="AD107" s="14" t="s">
+      <c r="AC107" s="14" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" s="14">
+        <f t="shared" si="68"/>
+        <v>1010</v>
+      </c>
+      <c r="G108" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
@@ -5459,18 +5487,51 @@
       <c r="N108" s="15"/>
       <c r="O108" s="15"/>
       <c r="P108" s="15"/>
-      <c r="Y108" s="16"/>
-    </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
-      <c r="Y109" s="12"/>
+      <c r="Q108" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R108" s="14" t="str">
+        <f t="shared" si="66"/>
+        <v>rm_optout_p1 Initial Stream</v>
+      </c>
+      <c r="S108" s="14" t="str">
+        <f t="shared" ref="S108" si="69">Q108</f>
+        <v>rm_optout_p1</v>
+      </c>
+      <c r="W108" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="X108" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y108" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD108" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="15"/>
+      <c r="M109" s="15"/>
+      <c r="N109" s="15"/>
+      <c r="O109" s="15"/>
+      <c r="P109" s="15"/>
+      <c r="Y109" s="16"/>
+    </row>
+    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+      <c r="M110" s="2"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Y110" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>